<commit_message>
Add pdf + xls/xlsx tests
</commit_message>
<xml_diff>
--- a/src/test/resources/files/1.xlsx
+++ b/src/test/resources/files/1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vasenkov\IdeaProjects\qa_guru_3_6\src\test\resources\html\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nedio\IdeaProjects\files\src\test\resources\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABDA9971-E665-42BB-B620-3D4CB00D26A7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BEF39D-911D-42D6-A0FA-7BB4798C0449}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8715" yWindow="-12990" windowWidth="21600" windowHeight="11385" xr2:uid="{60665258-6A6A-4099-A21A-8C7028A93874}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{60665258-6A6A-4099-A21A-8C7028A93874}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -23,10 +23,6 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,12 +30,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
-    <t>some text</t>
-  </si>
-  <si>
-    <t>hello qa.guru students!</t>
+    <t>test line</t>
   </si>
 </sst>
 </file>
@@ -402,21 +395,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E4FE8082-A083-4861-84C0-A3F9A56F40F1}">
-  <dimension ref="B4:B5"/>
+  <dimension ref="B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="4" spans="2:2">
       <c r="B4" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="2:2">
-      <c r="B5" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>